<commit_message>
Update Excel files from OneDrive - Wed May  7 06:35:43 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Line_Trials.xlsx
+++ b/data/Line_Trials.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B08585F4-3FD2-42D1-8839-48036BB71B86}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,7 +399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed May  7 15:58:57 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Line_Trials.xlsx
+++ b/data/Line_Trials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B046F7DF-DD4E-48E0-BEB2-34D4C24116CE}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{319DBB7C-2180-43C8-BBA4-E6F1D75BC3F0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{AD1C1EEB-A601-47B0-A44D-2CBCCAEDF7AF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{AD1C1EEB-A601-47B0-A44D-2CBCCAEDF7AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Material</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>order no.</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -747,7 +750,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -784,7 +787,27 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="D2" s="4"/>
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4">
+        <v>36892</v>
+      </c>
+      <c r="E2" s="4">
+        <v>36923</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Wed May  7 18:21:05 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Line_Trials.xlsx
+++ b/data/Line_Trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{319DBB7C-2180-43C8-BBA4-E6F1D75BC3F0}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E781B431-4B7C-483E-BA0F-F0A90D65404B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{AD1C1EEB-A601-47B0-A44D-2CBCCAEDF7AF}"/>
   </bookViews>
@@ -107,7 +107,7 @@
     <t>VENDOR</t>
   </si>
   <si>
-    <t>BOM UNDER TRIAL</t>
+    <t>BOM_UNDER_TRIAL</t>
   </si>
   <si>
     <t>STATUS</t>
@@ -122,7 +122,7 @@
     <t>REMARKS</t>
   </si>
   <si>
-    <t>order no.</t>
+    <t>ORDER_NO.</t>
   </si>
   <si>
     <t>ok</t>
@@ -216,12 +216,12 @@
   <autoFilter ref="A1:G1048576" xr:uid="{AB61B4F5-511E-49A9-92B3-D6FF18AC965A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{7A15D240-07DC-4EBC-BB7D-D8F8B01EC356}" name="VENDOR"/>
-    <tableColumn id="2" xr3:uid="{DD68DD6E-11AC-4E7A-A9ED-4F96706FB983}" name="BOM UNDER TRIAL"/>
+    <tableColumn id="2" xr3:uid="{DD68DD6E-11AC-4E7A-A9ED-4F96706FB983}" name="BOM_UNDER_TRIAL"/>
     <tableColumn id="3" xr3:uid="{45BA08C4-9760-4C25-88BD-E8B4213F6225}" name="STATUS"/>
     <tableColumn id="4" xr3:uid="{0F9BB0F7-18A2-4031-BC1D-7AFEEF0D905A}" name="START_DATE"/>
     <tableColumn id="5" xr3:uid="{0FE1B434-64DC-4EF2-B7A2-0EBA34772550}" name="END_DATE"/>
     <tableColumn id="6" xr3:uid="{9C1EA7EE-E918-4684-8D02-1D88FE7EEECF}" name="REMARKS"/>
-    <tableColumn id="7" xr3:uid="{D494BCEB-431B-446C-BBA5-C0D7D8A1C924}" name="order no."/>
+    <tableColumn id="7" xr3:uid="{D494BCEB-431B-446C-BBA5-C0D7D8A1C924}" name="ORDER_NO."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -750,7 +750,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon May 12 05:48:26 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Line_Trials.xlsx
+++ b/data/Line_Trials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28906"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E781B431-4B7C-483E-BA0F-F0A90D65404B}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{243D6A1B-E879-43BD-9E15-CD8B29413245}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{AD1C1EEB-A601-47B0-A44D-2CBCCAEDF7AF}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Material</t>
   </si>
@@ -125,7 +125,31 @@
     <t>ORDER_NO.</t>
   </si>
   <si>
-    <t>ok</t>
+    <t>PT NUSA SOLAR INDONESIA</t>
+  </si>
+  <si>
+    <t>SOLARCELL</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Dongguan CSG Solar Galss Co. L</t>
+  </si>
+  <si>
+    <t>TEMPERED GLASS</t>
+  </si>
+  <si>
+    <t>Zhejiang Jiaxing Taihe New Energy</t>
+  </si>
+  <si>
+    <t>AL FRAME LONG &amp; SHORT</t>
+  </si>
+  <si>
+    <t>Suzhou UKT New Energy Technology</t>
+  </si>
+  <si>
+    <t>JB SPLIT 1500V</t>
   </si>
 </sst>
 </file>
@@ -747,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41488953-EC08-4A94-828F-E576B84F7727}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -787,30 +811,91 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4">
-        <v>36892</v>
-      </c>
-      <c r="E2" s="4">
-        <v>36923</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
-        <v>27</v>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45782</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>22400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45782</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4">
+        <v>22400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45782</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5">
+        <v>22400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>45782</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6">
+        <v>22400</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{C65E90AC-94AD-469E-A23D-6321824390B1}">
       <formula1>Vendor_List</formula1>
     </dataValidation>
@@ -820,10 +905,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{D45427BD-053A-49EC-94BE-CA6B025BA066}">
       <formula1>Status_List</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E1048576" xr:uid="{59F8481F-015D-4063-BF15-D35056E76439}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 E2 E20:E1048576" xr:uid="{59F8481F-015D-4063-BF15-D35056E76439}">
       <formula1>36526</formula1>
       <formula2>73050</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E19" xr:uid="{7E0A543A-7176-4A6F-AB77-2C89CA9F9704}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon May 12 07:28:14 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Line_Trials.xlsx
+++ b/data/Line_Trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{243D6A1B-E879-43BD-9E15-CD8B29413245}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{853BBB71-229A-453A-A747-C08C2057B1A6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{AD1C1EEB-A601-47B0-A44D-2CBCCAEDF7AF}"/>
   </bookViews>
@@ -119,10 +119,10 @@
     <t>END_DATE</t>
   </si>
   <si>
-    <t>REMARKS</t>
-  </si>
-  <si>
     <t>ORDER_NO.</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
   <si>
     <t>PT NUSA SOLAR INDONESIA</t>
@@ -156,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +178,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFDC2626"/>
+      <name val="Roboto"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -212,12 +219,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,8 +252,8 @@
     <tableColumn id="3" xr3:uid="{45BA08C4-9760-4C25-88BD-E8B4213F6225}" name="STATUS"/>
     <tableColumn id="4" xr3:uid="{0F9BB0F7-18A2-4031-BC1D-7AFEEF0D905A}" name="START_DATE"/>
     <tableColumn id="5" xr3:uid="{0FE1B434-64DC-4EF2-B7A2-0EBA34772550}" name="END_DATE"/>
-    <tableColumn id="6" xr3:uid="{9C1EA7EE-E918-4684-8D02-1D88FE7EEECF}" name="REMARKS"/>
-    <tableColumn id="7" xr3:uid="{D494BCEB-431B-446C-BBA5-C0D7D8A1C924}" name="ORDER_NO."/>
+    <tableColumn id="6" xr3:uid="{9C1EA7EE-E918-4684-8D02-1D88FE7EEECF}" name="ORDER_NO."/>
+    <tableColumn id="7" xr3:uid="{D494BCEB-431B-446C-BBA5-C0D7D8A1C924}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -771,10 +779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41488953-EC08-4A94-828F-E576B84F7727}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -787,7 +795,7 @@
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -810,11 +818,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:11">
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -834,7 +842,7 @@
         <v>22400</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -854,7 +862,7 @@
         <v>22400</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -874,7 +882,7 @@
         <v>22400</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -893,6 +901,9 @@
       <c r="F6">
         <v>22400</v>
       </c>
+    </row>
+    <row r="7" spans="1:11" ht="15">
+      <c r="K7" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="5">

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-25 08:06:30
</commit_message>
<xml_diff>
--- a/data/Line_Trials.xlsx
+++ b/data/Line_Trials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.c\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{853BBB71-229A-453A-A747-C08C2057B1A6}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EED9F666-17FF-4185-A6FF-A26E4A6DD031}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{AD1C1EEB-A601-47B0-A44D-2CBCCAEDF7AF}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Material</t>
   </si>
@@ -107,9 +107,6 @@
     <t>VENDOR</t>
   </si>
   <si>
-    <t>BOM_UNDER_TRIAL</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -122,41 +119,27 @@
     <t>ORDER_NO.</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>PT NUSA SOLAR INDONESIA</t>
-  </si>
-  <si>
-    <t>SOLARCELL</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>Dongguan CSG Solar Galss Co. L</t>
-  </si>
-  <si>
-    <t>TEMPERED GLASS</t>
-  </si>
-  <si>
-    <t>Zhejiang Jiaxing Taihe New Energy</t>
-  </si>
-  <si>
-    <t>AL FRAME LONG &amp; SHORT</t>
-  </si>
-  <si>
-    <t>Suzhou UKT New Energy Technology</t>
-  </si>
-  <si>
-    <t>JB SPLIT 1500V</t>
+    <t>TRIAL</t>
+  </si>
+  <si>
+    <t>R&amp;D Production Order | G12R N-Type HEP Cell Line Trial | Comparison with
+regular 12R N-Type Cell</t>
+  </si>
+  <si>
+    <t>R&amp;D Production Order | Line trial of N-type M10 cells</t>
+  </si>
+  <si>
+    <t>GCL, URECO and JTPV</t>
+  </si>
+  <si>
+    <t>JTPV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,13 +202,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,16 +230,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB61B4F5-511E-49A9-92B3-D6FF18AC965A}" name="Table2" displayName="Table2" ref="A1:G1048576" totalsRowShown="0">
-  <autoFilter ref="A1:G1048576" xr:uid="{AB61B4F5-511E-49A9-92B3-D6FF18AC965A}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB61B4F5-511E-49A9-92B3-D6FF18AC965A}" name="Table2" displayName="Table2" ref="A1:F1048572" totalsRowShown="0">
+  <autoFilter ref="A1:F1048572" xr:uid="{AB61B4F5-511E-49A9-92B3-D6FF18AC965A}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7A15D240-07DC-4EBC-BB7D-D8F8B01EC356}" name="VENDOR"/>
-    <tableColumn id="2" xr3:uid="{DD68DD6E-11AC-4E7A-A9ED-4F96706FB983}" name="BOM_UNDER_TRIAL"/>
+    <tableColumn id="2" xr3:uid="{DD68DD6E-11AC-4E7A-A9ED-4F96706FB983}" name="TRIAL"/>
     <tableColumn id="3" xr3:uid="{45BA08C4-9760-4C25-88BD-E8B4213F6225}" name="STATUS"/>
     <tableColumn id="4" xr3:uid="{0F9BB0F7-18A2-4031-BC1D-7AFEEF0D905A}" name="START_DATE"/>
     <tableColumn id="5" xr3:uid="{0FE1B434-64DC-4EF2-B7A2-0EBA34772550}" name="END_DATE"/>
     <tableColumn id="6" xr3:uid="{9C1EA7EE-E918-4684-8D02-1D88FE7EEECF}" name="ORDER_NO."/>
-    <tableColumn id="7" xr3:uid="{D494BCEB-431B-446C-BBA5-C0D7D8A1C924}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -582,12 +567,12 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -617,7 +602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -632,7 +617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -647,7 +632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -662,7 +647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -675,7 +660,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -686,7 +671,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -697,7 +682,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -708,7 +693,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -717,7 +702,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -726,7 +711,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -735,7 +720,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -744,7 +729,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -753,7 +738,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -762,7 +747,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -779,148 +764,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41488953-EC08-4A94-828F-E576B84F7727}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.6328125" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="D2" s="4"/>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45918</v>
+      </c>
       <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="F2">
+        <v>23500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="4">
-        <v>45782</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
+        <v>45918</v>
       </c>
       <c r="F3">
-        <v>22400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45782</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4">
-        <v>22400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4">
-        <v>45782</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5">
-        <v>22400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4">
-        <v>45782</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6">
-        <v>22400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15">
-      <c r="K7" s="5"/>
+        <v>22420</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J7" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{C65E90AC-94AD-469E-A23D-6321824390B1}">
-      <formula1>Vendor_List</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{E19C66A5-A1AB-4E58-B499-4BCF53E1C31C}">
-      <formula1>Material_List</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{D45427BD-053A-49EC-94BE-CA6B025BA066}">
-      <formula1>Status_List</formula1>
-    </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 E2 E20:E1048576" xr:uid="{59F8481F-015D-4063-BF15-D35056E76439}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E16:E1048576 D2:D1048572" xr:uid="{59F8481F-015D-4063-BF15-D35056E76439}">
       <formula1>36526</formula1>
       <formula2>73050</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E19" xr:uid="{7E0A543A-7176-4A6F-AB77-2C89CA9F9704}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048572" xr:uid="{C65E90AC-94AD-469E-A23D-6321824390B1}">
+      <formula1>Vendor_List</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048572" xr:uid="{E19C66A5-A1AB-4E58-B499-4BCF53E1C31C}">
+      <formula1>Material_List</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048572" xr:uid="{D45427BD-053A-49EC-94BE-CA6B025BA066}">
+      <formula1>Status_List</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E15" xr:uid="{7E0A543A-7176-4A6F-AB77-2C89CA9F9704}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -933,5 +866,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C00D58-F8FB-4698-9B5A-4A446F07A6DA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C00D58-F8FB-4698-9B5A-4A446F07A6DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-25 09:42:32
</commit_message>
<xml_diff>
--- a/data/Line_Trials.xlsx
+++ b/data/Line_Trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EED9F666-17FF-4185-A6FF-A26E4A6DD031}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{638E6B0A-8B59-4A3A-A270-76F3326CB812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D14C59C7-AE4E-4CBD-8972-FC533E87DB58}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{AD1C1EEB-A601-47B0-A44D-2CBCCAEDF7AF}"/>
   </bookViews>
@@ -107,6 +107,9 @@
     <t>VENDOR</t>
   </si>
   <si>
+    <t>BOM_UNDER_TRIAL</t>
+  </si>
+  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -117,9 +120,6 @@
   </si>
   <si>
     <t>ORDER_NO.</t>
-  </si>
-  <si>
-    <t>TRIAL</t>
   </si>
   <si>
     <t>R&amp;D Production Order | G12R N-Type HEP Cell Line Trial | Comparison with
@@ -234,7 +234,7 @@
   <autoFilter ref="A1:F1048572" xr:uid="{AB61B4F5-511E-49A9-92B3-D6FF18AC965A}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{7A15D240-07DC-4EBC-BB7D-D8F8B01EC356}" name="VENDOR"/>
-    <tableColumn id="2" xr3:uid="{DD68DD6E-11AC-4E7A-A9ED-4F96706FB983}" name="TRIAL"/>
+    <tableColumn id="2" xr3:uid="{DD68DD6E-11AC-4E7A-A9ED-4F96706FB983}" name="BOM_UNDER_TRIAL"/>
     <tableColumn id="3" xr3:uid="{45BA08C4-9760-4C25-88BD-E8B4213F6225}" name="STATUS"/>
     <tableColumn id="4" xr3:uid="{0F9BB0F7-18A2-4031-BC1D-7AFEEF0D905A}" name="START_DATE"/>
     <tableColumn id="5" xr3:uid="{0FE1B434-64DC-4EF2-B7A2-0EBA34772550}" name="END_DATE"/>
@@ -767,7 +767,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -785,19 +785,19 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="58" x14ac:dyDescent="0.35">

</xml_diff>